<commit_message>
Signed-off-by: Hailemichael Nigussie <hailemichaeln@gmail.com>
</commit_message>
<xml_diff>
--- a/Site_Capacity.xlsx
+++ b/Site_Capacity.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40F10ED-BBEE-4582-BCA1-E4C34CFFD339}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="3465" yWindow="480" windowWidth="17025" windowHeight="9315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,7 +76,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmmyy"/>
   </numFmts>
@@ -508,11 +509,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T24" sqref="T24"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
'comment update, readme file update and exit code'
Signed-off-by: Hailemichael Nigussie <hailemichaeln@gmail.com>
</commit_message>
<xml_diff>
--- a/Site_Capacity.xlsx
+++ b/Site_Capacity.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40F10ED-BBEE-4582-BCA1-E4C34CFFD339}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4123F3-7C0B-4E4B-8CEC-55DD201E19EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="480" windowWidth="17025" windowHeight="9315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -512,13 +512,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="35.25" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -913,5 +913,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>